<commit_message>
CO: Finished classifying terms for CO DNR Guide to Well Permits and other legal things
</commit_message>
<xml_diff>
--- a/Vocabularies/CO/co-dnr-g2wr_g.xlsx
+++ b/Vocabularies/CO/co-dnr-g2wr_g.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/augustus/Desktop/WSWC/IoW/Vocabularies/CO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C569BD43-3582-8E42-8E63-1E4A31CCDBA7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80C9B39-DEBC-5746-8AD5-9CCB5EAE7E19}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3340" yWindow="760" windowWidth="31200" windowHeight="20000" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
+    <workbookView xWindow="3340" yWindow="760" windowWidth="31200" windowHeight="20000" activeTab="1" xr2:uid="{50A7F3F0-28DB-4FD5-8358-7DC84097337D}"/>
   </bookViews>
   <sheets>
     <sheet name="Vocabulary" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="145">
   <si>
     <t>Term</t>
   </si>
@@ -443,6 +443,24 @@
   </si>
   <si>
     <t>Any structure or device used for the purpose, or with the effect, of obtaining ground water for beneficial use from an aquifer. Additionally, any test hole or other excavation that is drilled, cored, bored, washed, fractured, driven, dug, jetted, or otherwise constructed, when the intended use of such excavation is for the location, monitoring, dewatering, observation, diversion, artificial recharge, or acquisition of ground water, or for conducting pumping equipment or aquifer tests.</t>
+  </si>
+  <si>
+    <t>Colorado Depatment of Natual Resources, Division of Water Resources</t>
+  </si>
+  <si>
+    <t>co-dnr</t>
+  </si>
+  <si>
+    <t>Guide to Colorado Well Permits, Water Rights and Water Administration</t>
+  </si>
+  <si>
+    <t>co-g2wr_g</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A glossary of terms from a 2012 guide on colorado well permits, water rights, and other related topics. </t>
+  </si>
+  <si>
+    <t>https://www.colorado.gov/pacific/sites/default/files/wellpermitguide_1.pdf</t>
   </si>
 </sst>
 </file>
@@ -821,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E542F74-ACD9-49CD-B312-AB6D05B8D550}">
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
@@ -1584,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251B0935-F8C3-480F-B897-E642A4205A23}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1626,6 +1644,24 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" t="s">
+        <v>144</v>
+      </c>
       <c r="G2" t="s">
         <v>26</v>
       </c>

</xml_diff>